<commit_message>
Added fan/fuel pump wiring
</commit_message>
<xml_diff>
--- a/ConnPinout.xlsx
+++ b/ConnPinout.xlsx
@@ -9,8 +9,7 @@
   </bookViews>
   <sheets>
     <sheet name="Connectors" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Splices" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Circut ID Naming" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Circut ID Naming" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -22,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="86">
   <si>
     <t xml:space="preserve">IC = inter connect</t>
   </si>
@@ -30,6 +29,12 @@
     <t xml:space="preserve">CC = component connector</t>
   </si>
   <si>
+    <t xml:space="preserve">PT = pigtail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RT = ring terminal</t>
+  </si>
+  <si>
     <t xml:space="preserve">R = receptacle</t>
   </si>
   <si>
@@ -129,10 +134,46 @@
     <t xml:space="preserve">BLACK</t>
   </si>
   <si>
+    <t xml:space="preserve">RT1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4BP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ICR1:1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5BP</t>
+  </si>
+  <si>
     <t xml:space="preserve">CCR2</t>
   </si>
   <si>
-    <t xml:space="preserve">S = splice</t>
+    <t xml:space="preserve">CCP5:2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2CT1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CCP6:2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2CT2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ICP1:11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CCP7:2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2CT3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CCP8:2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2CT4</t>
   </si>
   <si>
     <t xml:space="preserve">S1</t>
@@ -156,6 +197,9 @@
     <t xml:space="preserve">S2</t>
   </si>
   <si>
+    <t xml:space="preserve">ICP1:6</t>
+  </si>
+  <si>
     <t xml:space="preserve">CCP5:1</t>
   </si>
   <si>
@@ -213,10 +257,16 @@
     <t xml:space="preserve">Battery Ground</t>
   </si>
   <si>
+    <t xml:space="preserve">Fuel Pump</t>
+  </si>
+  <si>
     <t xml:space="preserve">CG</t>
   </si>
   <si>
     <t xml:space="preserve">Chassis Ground</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fan</t>
   </si>
   <si>
     <t xml:space="preserve">CT</t>
@@ -243,6 +293,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -264,17 +315,20 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="11"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -331,7 +385,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="18">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -344,7 +398,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -352,12 +406,16 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -372,10 +430,22 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -384,7 +454,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -465,17 +535,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F33"/>
+  <dimension ref="A1:F47"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
+      <pane xSplit="0" ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="5.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="5.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="10.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="10.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="9.59"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="5.88"/>
@@ -487,6 +559,7 @@
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
@@ -494,6 +567,7 @@
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
@@ -501,6 +575,7 @@
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
@@ -508,270 +583,483 @@
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="4" t="s">
+      <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="B8" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="C8" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="D8" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="5" t="s">
+      <c r="E8" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="1" t="n">
+      <c r="F8" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" s="2" t="s">
+      <c r="C9" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="5"/>
-      <c r="B8" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="C8" s="2" t="s">
+      <c r="D9" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="E9" s="2" t="s">
         <v>15</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="5"/>
-      <c r="B9" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="5"/>
       <c r="B10" s="1" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="5"/>
       <c r="B11" s="1" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="5"/>
       <c r="B12" s="1" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="5"/>
       <c r="B13" s="1" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="5"/>
       <c r="B14" s="1" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="5"/>
       <c r="B15" s="1" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="5"/>
       <c r="B16" s="1" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="5"/>
       <c r="B17" s="1" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="5"/>
       <c r="B18" s="1" t="n">
-        <v>12</v>
+        <v>10</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="5"/>
       <c r="B19" s="1" t="n">
-        <v>13</v>
+        <v>11</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="5"/>
       <c r="B20" s="1" t="n">
-        <v>14</v>
+        <v>12</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="5"/>
       <c r="B21" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E21" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="5"/>
       <c r="B22" s="1" t="n">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="5"/>
       <c r="B23" s="1" t="n">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="5"/>
       <c r="B24" s="1" t="n">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="5"/>
       <c r="B25" s="1" t="n">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="5"/>
       <c r="B26" s="1" t="n">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="5"/>
       <c r="B27" s="1" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="5"/>
+      <c r="B28" s="1" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="5"/>
+      <c r="B29" s="1" t="n">
         <v>21</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B29" s="1" t="n">
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B31" s="1" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="5"/>
-      <c r="B30" s="1" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="5"/>
-      <c r="B31" s="1" t="n">
-        <v>3</v>
+      <c r="C31" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="5"/>
       <c r="B32" s="1" t="n">
-        <v>4</v>
+        <v>2</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="5"/>
       <c r="B33" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="5"/>
+      <c r="B34" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="5"/>
+      <c r="B35" s="1" t="n">
         <v>5</v>
       </c>
+      <c r="C35" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B37" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E37" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="6"/>
+      <c r="B38" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C38" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E38" s="7"/>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="6"/>
+      <c r="B39" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="C39" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E39" s="7"/>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="6"/>
+      <c r="B40" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="C40" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E40" s="7"/>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="6"/>
+      <c r="B41" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="C41" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E41" s="7"/>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C42" s="7"/>
+      <c r="D42" s="1"/>
+      <c r="E42" s="7"/>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B43" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C43" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E43" s="7"/>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="6"/>
+      <c r="B44" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C44" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E44" s="7"/>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="6"/>
+      <c r="B45" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="C45" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E45" s="7"/>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="6"/>
+      <c r="B46" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="C46" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E46" s="7"/>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="6"/>
+      <c r="B47" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="C47" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E47" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="A7:A27"/>
-    <mergeCell ref="A29:A33"/>
+  <mergeCells count="10">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="A5:D5"/>
+    <mergeCell ref="A6:D6"/>
+    <mergeCell ref="A9:A29"/>
+    <mergeCell ref="A31:A35"/>
+    <mergeCell ref="A37:A41"/>
+    <mergeCell ref="A43:A47"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -788,342 +1076,173 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="5.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="8.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="9.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="8" width="4.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="9" width="19.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="9" width="1.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="7" width="5.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="7" width="18.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="7" width="1.39"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="B1" s="6"/>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="1" t="s">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="12"/>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="10"/>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="B3" s="13"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="E3" s="14"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="G4" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="8" t="n">
+        <v>2</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="G5" s="17"/>
+      <c r="H5" s="17"/>
+      <c r="I5" s="17"/>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="8" t="n">
+        <v>3</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="G6" s="17"/>
+      <c r="H6" s="17"/>
+      <c r="I6" s="17"/>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="8" t="n">
+        <v>4</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="G7" s="17"/>
+      <c r="H7" s="17"/>
+      <c r="I7" s="17"/>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="8" t="n">
         <v>5</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="B8" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="G8" s="17"/>
+      <c r="H8" s="17"/>
+      <c r="I8" s="17"/>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="8" t="n">
         <v>6</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D9" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="8" t="n">
         <v>7</v>
       </c>
-      <c r="E3" s="1" t="s">
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="8" t="n">
         <v>8</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="B4" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="D4" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="6"/>
-      <c r="B5" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="D5" s="1" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="6"/>
-      <c r="B6" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="D6" s="1" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="6"/>
-      <c r="B7" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="C7" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="D7" s="1" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="6"/>
-      <c r="B8" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="D8" s="1" t="n">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="B10" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="6"/>
-      <c r="B11" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="C11" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="D11" s="1" t="n">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="6"/>
-      <c r="B12" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="C12" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="D12" s="1" t="n">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="6"/>
-      <c r="B13" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="C13" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="D13" s="1" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="6"/>
-      <c r="B14" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="C14" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="D14" s="1" t="n">
-        <v>11</v>
-      </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A4:A8"/>
-    <mergeCell ref="A10:A14"/>
+  <mergeCells count="5">
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="G3:I3"/>
+    <mergeCell ref="G4:I8"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:G11"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="7" width="4.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="8" width="19.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="5.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.06"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="B1" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-    </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="9"/>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="B3" s="9"/>
-      <c r="C3" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="E4" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="7" t="n">
-        <v>2</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
-    </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="7" t="n">
-        <v>3</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="D6" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="13"/>
-    </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="7" t="n">
-        <v>4</v>
-      </c>
-      <c r="C7" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="D7" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="13"/>
-    </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="7" t="n">
-        <v>5</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="D8" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
-    </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="7" t="n">
-        <v>6</v>
-      </c>
-      <c r="C9" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="D9" s="0" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="7" t="n">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="7" t="n">
-        <v>8</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="E4:G8"/>
-  </mergeCells>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
Added wiring for ECT, IAT, TPS, MAP, EOP, O2 Sensor engine side, Cam/Crank engine side.
</commit_message>
<xml_diff>
--- a/ConnPinout.xlsx
+++ b/ConnPinout.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Connectors" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="132">
   <si>
     <t xml:space="preserve">IC = inter connect</t>
   </si>
@@ -146,6 +146,54 @@
     <t xml:space="preserve">5BP</t>
   </si>
   <si>
+    <t xml:space="preserve">S3:1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6AP2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S4:1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7AG1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GRAY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ICR5:1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8SI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ICR6:1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9SI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ICR2:1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10SI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ICR3:1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11SI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ICR4:1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12SI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NC</t>
+  </si>
+  <si>
     <t xml:space="preserve">CCR2</t>
   </si>
   <si>
@@ -212,6 +260,42 @@
     <t xml:space="preserve">CCP8:1</t>
   </si>
   <si>
+    <t xml:space="preserve">S3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ICP1:14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ICR2:2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ICR3:3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ICR4:2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ICR5:3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ICR6:3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ICP1:15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ICR3:2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ICR5:2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ICR6:2</t>
+  </si>
+  <si>
     <t xml:space="preserve">Ex</t>
   </si>
   <si>
@@ -269,16 +353,70 @@
     <t xml:space="preserve">Fan</t>
   </si>
   <si>
+    <t xml:space="preserve">AG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Analog Ground</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ECU_+5V</t>
+  </si>
+  <si>
     <t xml:space="preserve">CT</t>
   </si>
   <si>
     <t xml:space="preserve">Control</t>
   </si>
   <si>
-    <t xml:space="preserve">DA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Data</t>
+    <t xml:space="preserve">ECU_AGND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Digital Data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TPS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Signal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MAP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wire shielding</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ECT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EOP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IAT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Crank_VR+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Crank_VR-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cam_VR+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cam_VR-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O2 Sensor</t>
   </si>
 </sst>
 </file>
@@ -385,7 +523,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -407,10 +545,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -535,19 +669,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F47"/>
+  <dimension ref="A1:F59"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+      <selection pane="bottomLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="5.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="5.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="10.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="10.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="9.59"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="5.88"/>
@@ -799,61 +933,112 @@
       <c r="B22" s="1" t="n">
         <v>14</v>
       </c>
+      <c r="C22" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="5"/>
       <c r="B23" s="1" t="n">
         <v>15</v>
       </c>
+      <c r="C23" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="5"/>
       <c r="B24" s="1" t="n">
         <v>16</v>
       </c>
+      <c r="C24" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="5"/>
       <c r="B25" s="1" t="n">
         <v>17</v>
       </c>
+      <c r="C25" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="5"/>
       <c r="B26" s="1" t="n">
         <v>18</v>
       </c>
+      <c r="C26" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="5"/>
       <c r="B27" s="1" t="n">
         <v>19</v>
       </c>
+      <c r="C27" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="5"/>
       <c r="B28" s="1" t="n">
         <v>20</v>
       </c>
+      <c r="C28" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="5"/>
       <c r="B29" s="1" t="n">
         <v>21</v>
       </c>
+      <c r="C29" s="2" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="5" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="B31" s="1" t="n">
         <v>1</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>42</v>
+        <v>58</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>43</v>
+        <v>59</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -862,10 +1047,10 @@
         <v>2</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>44</v>
+        <v>60</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>45</v>
+        <v>61</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -874,7 +1059,7 @@
         <v>3</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>46</v>
+        <v>62</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>35</v>
@@ -889,10 +1074,10 @@
         <v>4</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>47</v>
+        <v>63</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>48</v>
+        <v>64</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -901,155 +1086,285 @@
         <v>5</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>49</v>
+        <v>65</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>50</v>
+        <v>66</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="6" t="s">
-        <v>51</v>
+      <c r="A37" s="5" t="s">
+        <v>67</v>
       </c>
       <c r="B37" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C37" s="7" t="s">
-        <v>52</v>
+      <c r="C37" s="6" t="s">
+        <v>68</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E37" s="7" t="s">
+      <c r="E37" s="6" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="6"/>
+      <c r="A38" s="5"/>
       <c r="B38" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C38" s="7" t="s">
-        <v>53</v>
+      <c r="C38" s="6" t="s">
+        <v>69</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E38" s="7"/>
+      <c r="E38" s="6"/>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="6"/>
+      <c r="A39" s="5"/>
       <c r="B39" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="C39" s="7" t="s">
-        <v>54</v>
+      <c r="C39" s="6" t="s">
+        <v>70</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E39" s="7"/>
+      <c r="E39" s="6"/>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="6"/>
+      <c r="A40" s="5"/>
       <c r="B40" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="C40" s="7" t="s">
-        <v>55</v>
+      <c r="C40" s="6" t="s">
+        <v>71</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E40" s="7"/>
+      <c r="E40" s="6"/>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="6"/>
+      <c r="A41" s="5"/>
       <c r="B41" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="C41" s="7" t="s">
-        <v>56</v>
+      <c r="C41" s="6" t="s">
+        <v>72</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E41" s="7"/>
+      <c r="E41" s="6"/>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C42" s="7"/>
+      <c r="C42" s="6"/>
       <c r="D42" s="1"/>
-      <c r="E42" s="7"/>
+      <c r="E42" s="6"/>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="6" t="s">
-        <v>57</v>
+      <c r="A43" s="5" t="s">
+        <v>73</v>
       </c>
       <c r="B43" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C43" s="7" t="s">
-        <v>58</v>
+      <c r="C43" s="6" t="s">
+        <v>74</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E43" s="7"/>
+      <c r="E43" s="6"/>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="6"/>
+      <c r="A44" s="5"/>
       <c r="B44" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C44" s="7" t="s">
-        <v>59</v>
+      <c r="C44" s="6" t="s">
+        <v>75</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E44" s="7"/>
+      <c r="E44" s="6"/>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="6"/>
+      <c r="A45" s="5"/>
       <c r="B45" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="C45" s="7" t="s">
-        <v>60</v>
+      <c r="C45" s="6" t="s">
+        <v>76</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E45" s="7"/>
+      <c r="E45" s="6"/>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="6"/>
+      <c r="A46" s="5"/>
       <c r="B46" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="C46" s="7" t="s">
-        <v>61</v>
+      <c r="C46" s="6" t="s">
+        <v>77</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E46" s="7"/>
+      <c r="E46" s="6"/>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="6"/>
+      <c r="A47" s="5"/>
       <c r="B47" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="C47" s="7" t="s">
-        <v>62</v>
+      <c r="C47" s="6" t="s">
+        <v>78</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E47" s="7"/>
+      <c r="E47" s="6"/>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B49" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C49" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="5"/>
+      <c r="B50" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C50" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="5"/>
+      <c r="B51" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="C51" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="5"/>
+      <c r="B52" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="C52" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="5"/>
+      <c r="B53" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="C53" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="5"/>
+      <c r="B54" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="C54" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="B56" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C56" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E56" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="5"/>
+      <c r="B57" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C57" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="5"/>
+      <c r="B58" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="C58" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="5"/>
+      <c r="B59" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="C59" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>44</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="12">
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="A3:D3"/>
@@ -1060,6 +1375,8 @@
     <mergeCell ref="A31:A35"/>
     <mergeCell ref="A37:A41"/>
     <mergeCell ref="A43:A47"/>
+    <mergeCell ref="A49:A54"/>
+    <mergeCell ref="A56:A59"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -1076,160 +1393,259 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A21" activeCellId="0" sqref="A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="8" width="4.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="9" width="19.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="9" width="1.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="7" width="5.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="7" width="18.06"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="7" width="1.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="7" width="4.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="8" width="19.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="8" width="1.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="6" width="5.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="6" width="18.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="6" width="1.39"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="B1" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="12"/>
+      <c r="A1" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="11"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="10"/>
+      <c r="A2" s="9"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="B3" s="13"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="E3" s="14"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
+      <c r="A3" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="B3" s="12"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="E3" s="13"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="H3" s="13"/>
+      <c r="I3" s="13"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="8" t="n">
+      <c r="A4" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="B4" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="D4" s="16" t="s">
-        <v>69</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="G4" s="17" t="s">
-        <v>71</v>
-      </c>
-      <c r="H4" s="17"/>
-      <c r="I4" s="17"/>
+      <c r="B4" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="G4" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="H4" s="16"/>
+      <c r="I4" s="16"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="8" t="n">
+      <c r="A5" s="7" t="n">
         <v>2</v>
       </c>
-      <c r="B5" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="D5" s="16" t="s">
-        <v>73</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="G5" s="17"/>
-      <c r="H5" s="17"/>
-      <c r="I5" s="17"/>
+      <c r="B5" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16"/>
+      <c r="I5" s="16"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="8" t="n">
+      <c r="A6" s="7" t="n">
         <v>3</v>
       </c>
-      <c r="B6" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="D6" s="16" t="s">
-        <v>76</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="G6" s="17"/>
-      <c r="H6" s="17"/>
-      <c r="I6" s="17"/>
+      <c r="B6" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="G6" s="16"/>
+      <c r="H6" s="16"/>
+      <c r="I6" s="16"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="8" t="n">
+      <c r="A7" s="7" t="n">
         <v>4</v>
       </c>
-      <c r="B7" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="D7" s="16" t="s">
-        <v>79</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="G7" s="17"/>
-      <c r="H7" s="17"/>
-      <c r="I7" s="17"/>
+      <c r="B7" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="G7" s="16"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="16"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="8" t="n">
+      <c r="A8" s="7" t="n">
         <v>5</v>
       </c>
-      <c r="B8" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="D8" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="G8" s="17"/>
-      <c r="H8" s="17"/>
-      <c r="I8" s="17"/>
+      <c r="B8" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="G8" s="16"/>
+      <c r="H8" s="16"/>
+      <c r="I8" s="16"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="8" t="n">
+      <c r="A9" s="7" t="n">
         <v>6</v>
       </c>
-      <c r="D9" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>85</v>
+      <c r="B9" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>113</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="8" t="n">
+      <c r="A10" s="7" t="n">
         <v>7</v>
       </c>
+      <c r="B10" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="8" t="n">
+      <c r="A11" s="7" t="n">
         <v>8</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="D11" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="7" t="n">
+        <v>9</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="D12" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="7" t="n">
+        <v>10</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="7" t="n">
+        <v>11</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="7" t="n">
+        <v>12</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="7" t="n">
+        <v>13</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="7" t="n">
+        <v>14</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="7" t="n">
+        <v>15</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="7" t="n">
+        <v>16</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="7" t="n">
+        <v>17</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>131</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added engine side shifter wiring. Started engine side power management wiring
</commit_message>
<xml_diff>
--- a/ConnPinout.xlsx
+++ b/ConnPinout.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="136">
   <si>
     <t xml:space="preserve">IC = inter connect</t>
   </si>
@@ -417,6 +417,18 @@
   </si>
   <si>
     <t xml:space="preserve">O2 Sensor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Up Shift</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Down Shift</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clutch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shift Solenoids</t>
   </si>
 </sst>
 </file>
@@ -672,12 +684,12 @@
   <dimension ref="A1:F59"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="8" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
+      <selection pane="bottomLeft" activeCell="C64" activeCellId="0" sqref="C64"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="5.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="5.6"/>
@@ -933,7 +945,7 @@
       <c r="B22" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="C22" s="0" t="s">
+      <c r="C22" s="6" t="s">
         <v>41</v>
       </c>
       <c r="D22" s="2" t="s">
@@ -948,7 +960,7 @@
       <c r="B23" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="C23" s="0" t="s">
+      <c r="C23" s="6" t="s">
         <v>43</v>
       </c>
       <c r="D23" s="2" t="s">
@@ -963,7 +975,7 @@
       <c r="B24" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="C24" s="0" t="s">
+      <c r="C24" s="6" t="s">
         <v>46</v>
       </c>
       <c r="D24" s="2" t="s">
@@ -975,7 +987,7 @@
       <c r="B25" s="1" t="n">
         <v>17</v>
       </c>
-      <c r="C25" s="0" t="s">
+      <c r="C25" s="6" t="s">
         <v>48</v>
       </c>
       <c r="D25" s="2" t="s">
@@ -987,7 +999,7 @@
       <c r="B26" s="1" t="n">
         <v>18</v>
       </c>
-      <c r="C26" s="0" t="s">
+      <c r="C26" s="6" t="s">
         <v>50</v>
       </c>
       <c r="D26" s="2" t="s">
@@ -999,7 +1011,7 @@
       <c r="B27" s="1" t="n">
         <v>19</v>
       </c>
-      <c r="C27" s="0" t="s">
+      <c r="C27" s="6" t="s">
         <v>52</v>
       </c>
       <c r="D27" s="2" t="s">
@@ -1011,7 +1023,7 @@
       <c r="B28" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="C28" s="0" t="s">
+      <c r="C28" s="6" t="s">
         <v>54</v>
       </c>
       <c r="D28" s="2" t="s">
@@ -1393,13 +1405,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I20"/>
+  <dimension ref="A1:I33"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A21" activeCellId="0" sqref="A21"/>
+      <selection pane="topLeft" activeCell="B25" activeCellId="0" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="7" width="4.97"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="8" width="19.17"/>
@@ -1646,6 +1658,83 @@
       </c>
       <c r="B20" s="8" t="s">
         <v>131</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="7" t="n">
+        <v>18</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="7" t="n">
+        <v>19</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="7" t="n">
+        <v>20</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="7" t="n">
+        <v>21</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="7" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="7" t="n">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="7" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="7" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="7" t="n">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="7" t="n">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="7" t="n">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="7" t="n">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="7" t="n">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added shifter, brake light wiring, organized pwr mgmt diagrams
</commit_message>
<xml_diff>
--- a/ConnPinout.xlsx
+++ b/ConnPinout.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Connectors" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="156">
   <si>
     <t xml:space="preserve">IC = inter connect</t>
   </si>
@@ -41,6 +41,9 @@
     <t xml:space="preserve">P = plug</t>
   </si>
   <si>
+    <t xml:space="preserve">SH = shield</t>
+  </si>
+  <si>
     <t xml:space="preserve">Ref</t>
   </si>
   <si>
@@ -140,7 +143,7 @@
     <t xml:space="preserve">4BP</t>
   </si>
   <si>
-    <t xml:space="preserve">ICR1:1</t>
+    <t xml:space="preserve">ICR7:1</t>
   </si>
   <si>
     <t xml:space="preserve">5BP</t>
@@ -191,7 +194,58 @@
     <t xml:space="preserve">12SI</t>
   </si>
   <si>
-    <t xml:space="preserve">NC</t>
+    <t xml:space="preserve">ICP6:1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22SI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ICR1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13SI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14SI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13SH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ICP2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15SI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16SI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15SH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ICR8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21BP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18CT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">19CT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ICR9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20CT</t>
   </si>
   <si>
     <t xml:space="preserve">CCR2</t>
@@ -296,6 +350,12 @@
     <t xml:space="preserve">ICR6:2</t>
   </si>
   <si>
+    <t xml:space="preserve">ICR9:1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ICR8:1</t>
+  </si>
+  <si>
     <t xml:space="preserve">Ex</t>
   </si>
   <si>
@@ -389,9 +449,6 @@
     <t xml:space="preserve">MAP</t>
   </si>
   <si>
-    <t xml:space="preserve">SH</t>
-  </si>
-  <si>
     <t xml:space="preserve">Wire shielding</t>
   </si>
   <si>
@@ -429,6 +486,9 @@
   </si>
   <si>
     <t xml:space="preserve">Shift Solenoids</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brake Light</t>
   </si>
 </sst>
 </file>
@@ -535,7 +595,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -562,6 +622,18 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -677,25 +749,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F59"/>
+  <dimension ref="A1:F79"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="8" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="8" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C64" activeCellId="0" sqref="C64"/>
+      <selection pane="bottomLeft" activeCell="E31" activeCellId="0" sqref="E31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="5.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="5.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="10.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="9.59"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="9.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="5.88"/>
   </cols>
   <sheetData>
@@ -747,648 +819,818 @@
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
     </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="4" t="s">
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="B9" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="C9" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="D9" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="E9" s="4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="5" t="s">
+      <c r="F9" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="1" t="n">
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9" s="2" t="s">
+      <c r="C10" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="D10" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="5"/>
-      <c r="B10" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="C10" s="2" t="s">
+      <c r="E10" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="5"/>
       <c r="B11" s="1" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C11" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="5"/>
       <c r="B12" s="1" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C12" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="5"/>
       <c r="B13" s="1" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C13" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="5"/>
       <c r="B14" s="1" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C14" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>24</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="5"/>
       <c r="B15" s="1" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C15" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D15" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D15" s="2" t="s">
-        <v>27</v>
+      <c r="E15" s="2" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="5"/>
       <c r="B16" s="1" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C16" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D16" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="5"/>
       <c r="B17" s="1" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C17" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D17" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="5"/>
       <c r="B18" s="1" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C18" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D18" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="5"/>
       <c r="B19" s="1" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C19" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D19" s="2" t="s">
         <v>34</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="5"/>
       <c r="B20" s="1" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C20" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E20" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="5"/>
       <c r="B21" s="1" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C21" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D21" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D21" s="2" t="s">
-        <v>40</v>
-      </c>
       <c r="E21" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="5"/>
       <c r="B22" s="1" t="n">
-        <v>14</v>
-      </c>
-      <c r="C22" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D22" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D22" s="2" t="s">
-        <v>42</v>
-      </c>
       <c r="E22" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="5"/>
       <c r="B23" s="1" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C23" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D23" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D23" s="2" t="s">
-        <v>44</v>
-      </c>
       <c r="E23" s="2" t="s">
-        <v>45</v>
+        <v>16</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="5"/>
       <c r="B24" s="1" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C24" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E24" s="2" t="s">
         <v>46</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="5"/>
       <c r="B25" s="1" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C25" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D25" s="2" t="s">
         <v>48</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="5"/>
       <c r="B26" s="1" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C26" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="D26" s="2" t="s">
         <v>50</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="5"/>
       <c r="B27" s="1" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C27" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D27" s="2" t="s">
         <v>52</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="5"/>
       <c r="B28" s="1" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C28" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D28" s="2" t="s">
         <v>54</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="5"/>
       <c r="B29" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="5"/>
+      <c r="B30" s="1" t="n">
         <v>21</v>
       </c>
-      <c r="C29" s="2" t="s">
-        <v>56</v>
+      <c r="C30" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="B31" s="1" t="n">
+      <c r="A31" s="7"/>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B32" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C31" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="5"/>
-      <c r="B32" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="C32" s="2" t="s">
+      <c r="D32" s="2" t="s">
         <v>60</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="5"/>
       <c r="B33" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>62</v>
+        <v>2</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>36</v>
+        <v>61</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="5"/>
-      <c r="B34" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="C34" s="2" t="s">
+      <c r="B34" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D34" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="D34" s="2" t="s">
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="7"/>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="5" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="5"/>
-      <c r="B35" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="C35" s="2" t="s">
+      <c r="B36" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D36" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="D35" s="2" t="s">
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="5"/>
+      <c r="B37" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="D37" s="2" t="s">
         <v>66</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="B37" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="C37" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E37" s="6" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="5"/>
-      <c r="B38" s="1" t="n">
+      <c r="B38" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="B40" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="8"/>
+      <c r="B41" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C38" s="6" t="s">
+      <c r="D41" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="8"/>
+      <c r="B42" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="B44" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C44" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="D38" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E38" s="6"/>
-    </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="5"/>
-      <c r="B39" s="1" t="n">
+      <c r="D44" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="8"/>
+      <c r="B45" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B47" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="5"/>
+      <c r="B48" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="5"/>
+      <c r="B49" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="C39" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E39" s="6"/>
-    </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="5"/>
-      <c r="B40" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="C40" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E40" s="6"/>
-    </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="5"/>
-      <c r="B41" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="C41" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E41" s="6"/>
-    </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C42" s="6"/>
-      <c r="D42" s="1"/>
-      <c r="E42" s="6"/>
-    </row>
-    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="B43" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="C43" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E43" s="6"/>
-    </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="5"/>
-      <c r="B44" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="C44" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E44" s="6"/>
-    </row>
-    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="5"/>
-      <c r="B45" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="C45" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E45" s="6"/>
-    </row>
-    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="5"/>
-      <c r="B46" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="C46" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E46" s="6"/>
-    </row>
-    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="5"/>
-      <c r="B47" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="C47" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E47" s="6"/>
-    </row>
-    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="B49" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="C49" s="6" t="s">
+      <c r="C49" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="D49" s="1" t="s">
-        <v>42</v>
+      <c r="D49" s="2" t="s">
+        <v>36</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>15</v>
+        <v>37</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="5"/>
       <c r="B50" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="C50" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C50" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="D50" s="1" t="s">
-        <v>42</v>
+      <c r="D50" s="2" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="5"/>
       <c r="B51" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="C51" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="5"/>
-      <c r="B52" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="C52" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C51" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="D52" s="1" t="s">
-        <v>42</v>
+      <c r="D51" s="2" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="5"/>
+      <c r="A53" s="5" t="s">
+        <v>85</v>
+      </c>
       <c r="B53" s="1" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C53" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>42</v>
+        <v>86</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E53" s="9" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="5"/>
       <c r="B54" s="1" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C54" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>42</v>
-      </c>
+        <v>87</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E54" s="9"/>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="5"/>
+      <c r="B55" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="C55" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E55" s="9"/>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="5" t="s">
-        <v>86</v>
-      </c>
+      <c r="A56" s="5"/>
       <c r="B56" s="1" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C56" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="E56" s="2" t="s">
-        <v>45</v>
-      </c>
+        <v>89</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E56" s="9"/>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="5"/>
       <c r="B57" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="C57" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E57" s="9"/>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C58" s="6"/>
+      <c r="E58" s="9"/>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="B59" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C59" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E59" s="9"/>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="5"/>
+      <c r="B60" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C57" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="5"/>
-      <c r="B58" s="1" t="n">
+      <c r="C60" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E60" s="9"/>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="5"/>
+      <c r="B61" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="C58" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="5"/>
-      <c r="B59" s="1" t="n">
+      <c r="C61" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E61" s="9"/>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="5"/>
+      <c r="B62" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="C59" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="D59" s="1" t="s">
-        <v>44</v>
+      <c r="C62" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E62" s="9"/>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="5"/>
+      <c r="B63" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="C63" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E63" s="9"/>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="B65" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C65" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="D65" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E65" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="5"/>
+      <c r="B66" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C66" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="D66" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="5"/>
+      <c r="B67" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="C67" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="D67" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="5"/>
+      <c r="B68" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="C68" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="D68" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="5"/>
+      <c r="B69" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="C69" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="5"/>
+      <c r="B70" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="C70" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="B72" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C72" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E72" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="5"/>
+      <c r="B73" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C73" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="5"/>
+      <c r="B74" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="C74" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="5"/>
+      <c r="B75" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="C75" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B77" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D77" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="5"/>
+      <c r="B78" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D78" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="5"/>
+      <c r="B79" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="D79" s="2" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="18">
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="A3:D3"/>
     <mergeCell ref="A4:D4"/>
     <mergeCell ref="A5:D5"/>
     <mergeCell ref="A6:D6"/>
-    <mergeCell ref="A9:A29"/>
-    <mergeCell ref="A31:A35"/>
-    <mergeCell ref="A37:A41"/>
-    <mergeCell ref="A43:A47"/>
-    <mergeCell ref="A49:A54"/>
-    <mergeCell ref="A56:A59"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="A10:A30"/>
+    <mergeCell ref="A32:A34"/>
+    <mergeCell ref="A36:A38"/>
+    <mergeCell ref="A40:A42"/>
+    <mergeCell ref="A44:A45"/>
+    <mergeCell ref="A47:A51"/>
+    <mergeCell ref="A53:A57"/>
+    <mergeCell ref="A59:A63"/>
+    <mergeCell ref="A65:A70"/>
+    <mergeCell ref="A72:A75"/>
+    <mergeCell ref="A77:A79"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -1401,339 +1643,342 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B25" activeCellId="0" sqref="B25"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B26" activeCellId="0" sqref="B26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="7" width="4.97"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="8" width="19.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="8" width="1.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="10" width="4.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="11" width="19.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="11" width="1.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="6" width="5.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="6" width="18.06"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="6" width="1.39"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="B1" s="10" t="s">
-        <v>92</v>
-      </c>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="11"/>
+      <c r="A1" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="14"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="9"/>
+      <c r="A2" s="12"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="12" t="s">
-        <v>93</v>
-      </c>
-      <c r="B3" s="12"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="13" t="s">
-        <v>94</v>
-      </c>
-      <c r="E3" s="13"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="13" t="s">
-        <v>95</v>
-      </c>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
+      <c r="A3" s="15" t="s">
+        <v>113</v>
+      </c>
+      <c r="B3" s="15"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="E3" s="16"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="H3" s="16"/>
+      <c r="I3" s="16"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="7" t="n">
+      <c r="A4" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="B4" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="D4" s="15" t="s">
-        <v>97</v>
+      <c r="B4" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>117</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="G4" s="16" t="s">
-        <v>99</v>
-      </c>
-      <c r="H4" s="16"/>
-      <c r="I4" s="16"/>
+        <v>118</v>
+      </c>
+      <c r="G4" s="19" t="s">
+        <v>119</v>
+      </c>
+      <c r="H4" s="19"/>
+      <c r="I4" s="19"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="7" t="n">
+      <c r="A5" s="10" t="n">
         <v>2</v>
       </c>
-      <c r="B5" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="D5" s="15" t="s">
-        <v>101</v>
+      <c r="B5" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="D5" s="18" t="s">
+        <v>121</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="G5" s="16"/>
-      <c r="H5" s="16"/>
-      <c r="I5" s="16"/>
+        <v>122</v>
+      </c>
+      <c r="G5" s="19"/>
+      <c r="H5" s="19"/>
+      <c r="I5" s="19"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="7" t="n">
+      <c r="A6" s="10" t="n">
         <v>3</v>
       </c>
-      <c r="B6" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="D6" s="15" t="s">
-        <v>104</v>
+      <c r="B6" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>124</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="G6" s="16"/>
-      <c r="H6" s="16"/>
-      <c r="I6" s="16"/>
+        <v>125</v>
+      </c>
+      <c r="G6" s="19"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="19"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="7" t="n">
+      <c r="A7" s="10" t="n">
         <v>4</v>
       </c>
-      <c r="B7" s="8" t="s">
-        <v>106</v>
-      </c>
-      <c r="D7" s="15" t="s">
-        <v>107</v>
+      <c r="B7" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="D7" s="18" t="s">
+        <v>127</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="G7" s="16"/>
-      <c r="H7" s="16"/>
-      <c r="I7" s="16"/>
+        <v>128</v>
+      </c>
+      <c r="G7" s="19"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="19"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="7" t="n">
+      <c r="A8" s="10" t="n">
         <v>5</v>
       </c>
-      <c r="B8" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="D8" s="15" t="s">
-        <v>110</v>
+      <c r="B8" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>130</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="G8" s="16"/>
-      <c r="H8" s="16"/>
-      <c r="I8" s="16"/>
+        <v>131</v>
+      </c>
+      <c r="G8" s="19"/>
+      <c r="H8" s="19"/>
+      <c r="I8" s="19"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="7" t="n">
+      <c r="A9" s="10" t="n">
         <v>6</v>
       </c>
-      <c r="B9" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="D9" s="15" t="s">
-        <v>113</v>
+      <c r="B9" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="D9" s="18" t="s">
+        <v>133</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>114</v>
+        <v>134</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="7" t="n">
+      <c r="A10" s="10" t="n">
         <v>7</v>
       </c>
-      <c r="B10" s="8" t="s">
-        <v>115</v>
-      </c>
-      <c r="D10" s="15" t="s">
-        <v>116</v>
+      <c r="B10" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="D10" s="18" t="s">
+        <v>136</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>117</v>
+        <v>137</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="7" t="n">
+      <c r="A11" s="10" t="n">
         <v>8</v>
       </c>
-      <c r="B11" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="D11" s="15" t="s">
-        <v>119</v>
+      <c r="B11" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="D11" s="18" t="s">
+        <v>139</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>120</v>
+        <v>140</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="7" t="n">
+      <c r="A12" s="10" t="n">
         <v>9</v>
       </c>
-      <c r="B12" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="D12" s="15" t="s">
-        <v>122</v>
+      <c r="B12" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="D12" s="18" t="s">
+        <v>62</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>123</v>
+        <v>142</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="7" t="n">
+      <c r="A13" s="10" t="n">
         <v>10</v>
       </c>
-      <c r="B13" s="8" t="s">
-        <v>124</v>
+      <c r="B13" s="11" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="7" t="n">
+      <c r="A14" s="10" t="n">
         <v>11</v>
       </c>
-      <c r="B14" s="8" t="s">
-        <v>125</v>
+      <c r="B14" s="11" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="7" t="n">
+      <c r="A15" s="10" t="n">
         <v>12</v>
       </c>
-      <c r="B15" s="8" t="s">
-        <v>126</v>
+      <c r="B15" s="11" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="7" t="n">
+      <c r="A16" s="10" t="n">
         <v>13</v>
       </c>
-      <c r="B16" s="8" t="s">
-        <v>127</v>
+      <c r="B16" s="11" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="7" t="n">
+      <c r="A17" s="10" t="n">
         <v>14</v>
       </c>
-      <c r="B17" s="8" t="s">
-        <v>128</v>
+      <c r="B17" s="11" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="7" t="n">
+      <c r="A18" s="10" t="n">
         <v>15</v>
       </c>
-      <c r="B18" s="8" t="s">
-        <v>129</v>
+      <c r="B18" s="11" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="7" t="n">
+      <c r="A19" s="10" t="n">
         <v>16</v>
       </c>
-      <c r="B19" s="8" t="s">
-        <v>130</v>
+      <c r="B19" s="11" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="7" t="n">
+      <c r="A20" s="10" t="n">
         <v>17</v>
       </c>
-      <c r="B20" s="8" t="s">
-        <v>131</v>
+      <c r="B20" s="11" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="7" t="n">
+      <c r="A21" s="10" t="n">
         <v>18</v>
       </c>
-      <c r="B21" s="8" t="s">
-        <v>132</v>
+      <c r="B21" s="11" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="7" t="n">
+      <c r="A22" s="10" t="n">
         <v>19</v>
       </c>
-      <c r="B22" s="8" t="s">
-        <v>133</v>
+      <c r="B22" s="11" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="7" t="n">
+      <c r="A23" s="10" t="n">
         <v>20</v>
       </c>
-      <c r="B23" s="8" t="s">
-        <v>134</v>
+      <c r="B23" s="11" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="7" t="n">
+      <c r="A24" s="10" t="n">
         <v>21</v>
       </c>
-      <c r="B24" s="8" t="s">
-        <v>135</v>
+      <c r="B24" s="11" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="7" t="n">
+      <c r="A25" s="10" t="n">
         <v>22</v>
       </c>
+      <c r="B25" s="11" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="7" t="n">
+      <c r="A26" s="10" t="n">
         <v>23</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="7" t="n">
+      <c r="A27" s="10" t="n">
         <v>24</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="7" t="n">
+      <c r="A28" s="10" t="n">
         <v>25</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="7" t="n">
+      <c r="A29" s="10" t="n">
         <v>26</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="7" t="n">
+      <c r="A30" s="10" t="n">
         <v>27</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="7" t="n">
+      <c r="A31" s="10" t="n">
         <v>28</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="7" t="n">
+      <c r="A32" s="10" t="n">
         <v>29</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="7" t="n">
+      <c r="A33" s="10" t="n">
         <v>30</v>
       </c>
     </row>

</xml_diff>